<commit_message>
update description of linear regression
</commit_message>
<xml_diff>
--- a/output/Data_Reduction.xlsx
+++ b/output/Data_Reduction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\toothheart\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\cvd-and-teeth\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B406036D-AA5C-47E0-914D-7945BA2C8154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D73F342-B20D-4694-BDFD-69D24C0258C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21780" yWindow="-15870" windowWidth="15555" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Exclusion</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Know teeth removed</t>
+  </si>
+  <si>
+    <t>% of Start</t>
+  </si>
+  <si>
+    <t>% of Subpopulation</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -235,13 +241,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,9 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -982,7 +992,10 @@
     <col min="2" max="2" width="27.7109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="15"/>
+    <col min="5" max="5" width="9.140625" style="15"/>
+    <col min="6" max="6" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -998,6 +1011,12 @@
       <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
@@ -1029,6 +1048,14 @@
       <c r="D3" s="14">
         <v>274309</v>
       </c>
+      <c r="F3" s="22">
+        <f>C3/A$2</f>
+        <v>3.5388033906674347E-3</v>
+      </c>
+      <c r="G3" s="22">
+        <f>C3/A$3</f>
+        <v>5.6116031132072055E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
@@ -1044,6 +1071,14 @@
       </c>
       <c r="D4" s="14">
         <v>266109</v>
+      </c>
+      <c r="F4" s="22">
+        <f>C4/A$2</f>
+        <v>1.8745599356248685E-2</v>
+      </c>
+      <c r="G4" s="22">
+        <f>C4/A$3</f>
+        <v>2.9725546206911552E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1062,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
@@ -1085,7 +1120,7 @@
       <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
@@ -1095,7 +1130,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
-      <c r="C4" s="18"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="7"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1106,7 +1141,7 @@
         <f>"n = "&amp;TEXT(Worksheet!A2,"#,###")</f>
         <v>n = 437,436</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="8" t="str">
         <f>"n = "&amp;TEXT(Worksheet!C2,"#,###")</f>
         <v>n = 161,579</v>
@@ -1145,7 +1180,7 @@
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1155,7 +1190,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
-      <c r="C10" s="18"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="7"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1166,7 +1201,7 @@
         <f>"n = "&amp;TEXT(Worksheet!D2,"#,###")</f>
         <v>n = 275,857</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="8" t="str">
         <f>"n = "&amp;TEXT(Worksheet!C3,"#,###")</f>
         <v>n = 1,548</v>
@@ -1203,7 +1238,7 @@
       <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="11" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1248,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
-      <c r="C16" s="18"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="7"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1224,7 +1259,7 @@
         <f>"n = "&amp;TEXT(Worksheet!D3,"#,###")</f>
         <v>n = 274,309</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="8" t="str">
         <f>"n = "&amp;TEXT(Worksheet!C4,"#,###")</f>
         <v>n = 8,200</v>
@@ -1251,18 +1286,18 @@
     </row>
     <row r="20" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="D20" s="19"/>
+      <c r="D20" s="18"/>
     </row>
     <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="17"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="18"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1270,8 +1305,8 @@
         <f>"n = "&amp;TEXT(Worksheet!D4,"#,###")</f>
         <v>n = 266,109</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="19"/>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>

</xml_diff>